<commit_message>
Added extra columns to template
</commit_message>
<xml_diff>
--- a/storage/templates/recipient_template.xlsx
+++ b/storage/templates/recipient_template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Recipient Name</t>
   </si>
@@ -36,6 +36,21 @@
   </si>
   <si>
     <t>example@recipient.com</t>
+  </si>
+  <si>
+    <t>Is Business Owner/Company Employee</t>
+  </si>
+  <si>
+    <t>Business/Company Name</t>
+  </si>
+  <si>
+    <t>Business/Company Position</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>Template Co. Inc</t>
   </si>
 </sst>
 </file>
@@ -359,30 +374,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.5" customWidth="1"/>
     <col min="2" max="2" width="43.5" customWidth="1"/>
+    <col min="3" max="3" width="34.5" customWidth="1"/>
+    <col min="4" max="4" width="40.1640625" customWidth="1"/>
+    <col min="5" max="5" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>